<commit_message>
update website coloring, edit poster
</commit_message>
<xml_diff>
--- a/docs/eg_data/NHANES/PF/10_KCAL means.xlsx
+++ b/docs/eg_data/NHANES/PF/10_KCAL means.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadoh\OneDrive\Documents\GitHub\DietR\eg_data\NHANES\PF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ABC272B-E964-447B-A667-4E89B4ED4852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26619361-668C-479D-A528-14BFB3C430E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5985" yWindow="615" windowWidth="13500" windowHeight="10020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KCAL" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="80">
   <si>
     <t>Plain means</t>
   </si>
@@ -588,6 +591,331 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.26583506859585976"/>
+          <c:y val="6.7276620684465105E-2"/>
+          <c:w val="0.69848926180221127"/>
+          <c:h val="0.76845122306270808"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>KCAL!$T$133</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>emmean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>KCAL!$M$134:$M$137</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>13.6563338055635</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>16.4368928850663</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>30.334330472387201</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>31.174938955120801</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>KCAL!$M$134:$M$137</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>13.6563338055635</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>16.4368928850663</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>30.334330472387201</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>31.174938955120801</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>KCAL!$S$134:$S$137</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>DivNA</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Div0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Div1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Div2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>KCAL!$T$134:$T$137</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1977.15672849103</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2020.70670468556</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2088.00107638999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2151.7802221952802</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-46EE-47B0-903B-DC1BFE466511}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="134"/>
+        <c:overlap val="-45"/>
+        <c:axId val="477875424"/>
+        <c:axId val="477873624"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="477875424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="65000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="477873624"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="477873624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="477875424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="65000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1600">
+          <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1026,7 +1354,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1568,7 +1896,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2151,19 +2479,59 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinearReversed" id="21">
   <a:schemeClr val="accent1"/>
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinearReversed" id="26">
   <a:schemeClr val="accent6"/>
 </cs:colorStyle>
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -3169,6 +3537,509 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3761,10 +4632,114 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>534459</xdr:colOff>
+      <xdr:row>146</xdr:row>
+      <xdr:rowOff>62441</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15262AAC-7F9E-471F-824B-3345F7EA2A23}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>2.55373E-7</cdr:x>
+      <cdr:y>0.01167</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.1</cdr:x>
+      <cdr:y>0.89883</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{855F7DC9-3DD0-48DB-EA7D-4FA42F8645E7}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="16200000">
+          <a:off x="-1010712" y="1042454"/>
+          <a:ext cx="2413009" cy="391583"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>KCAL</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1050">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4049,6 +5024,80 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="149">
+          <cell r="T149" t="str">
+            <v>emmean</v>
+          </cell>
+        </row>
+        <row r="150">
+          <cell r="S150" t="str">
+            <v>DivNA</v>
+          </cell>
+          <cell r="T150">
+            <v>29.833039894761601</v>
+          </cell>
+        </row>
+        <row r="151">
+          <cell r="S151" t="str">
+            <v>Div0</v>
+          </cell>
+          <cell r="T151">
+            <v>29.701989237987501</v>
+          </cell>
+        </row>
+        <row r="152">
+          <cell r="S152" t="str">
+            <v>Div1</v>
+          </cell>
+          <cell r="T152">
+            <v>28.923320343383399</v>
+          </cell>
+        </row>
+        <row r="153">
+          <cell r="S153" t="str">
+            <v>Div2</v>
+          </cell>
+          <cell r="T153">
+            <v>27.695775047685299</v>
+          </cell>
+        </row>
+        <row r="160">
+          <cell r="D160">
+            <v>0.165029993120519</v>
+          </cell>
+        </row>
+        <row r="161">
+          <cell r="D161">
+            <v>0.198631664864556</v>
+          </cell>
+        </row>
+        <row r="162">
+          <cell r="D162">
+            <v>0.36657527711677601</v>
+          </cell>
+        </row>
+        <row r="163">
+          <cell r="D163">
+            <v>0.37673361200355499</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4312,10 +5361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q154"/>
+  <dimension ref="A1:T154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A143" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A153" sqref="A153"/>
+    <sheetView tabSelected="1" topLeftCell="C120" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q140" sqref="K140:Q140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6370,7 +7419,7 @@
         <v>&lt;0.0001</v>
       </c>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
         <v>71</v>
       </c>
@@ -6403,7 +7452,7 @@
         <v>&lt;0.0001</v>
       </c>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
         <v>75</v>
       </c>
@@ -6436,7 +7485,7 @@
         <v>&lt;0.0001</v>
       </c>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B131" s="5" t="s">
         <v>66</v>
       </c>
@@ -6468,7 +7517,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
         <v>5</v>
       </c>
@@ -6517,8 +7566,14 @@
       <c r="Q133" s="5" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S133" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="T133" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="134" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>1</v>
       </c>
@@ -6567,8 +7622,14 @@
       <c r="Q134" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S134" t="s">
+        <v>1</v>
+      </c>
+      <c r="T134" s="1">
+        <v>1977.15672849103</v>
+      </c>
+    </row>
+    <row r="135" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>2</v>
       </c>
@@ -6617,8 +7678,14 @@
       <c r="Q135" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S135" t="s">
+        <v>2</v>
+      </c>
+      <c r="T135" s="1">
+        <v>2020.70670468556</v>
+      </c>
+    </row>
+    <row r="136" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>3</v>
       </c>
@@ -6667,8 +7734,14 @@
       <c r="Q136" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S136" t="s">
+        <v>3</v>
+      </c>
+      <c r="T136" s="1">
+        <v>2088.00107638999</v>
+      </c>
+    </row>
+    <row r="137" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>4</v>
       </c>
@@ -6717,8 +7790,14 @@
       <c r="Q137" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S137" t="s">
+        <v>4</v>
+      </c>
+      <c r="T137" s="1">
+        <v>2151.7802221952802</v>
+      </c>
+    </row>
+    <row r="138" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>13</v>
       </c>
@@ -6769,7 +7848,7 @@
         <v>0.186</v>
       </c>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>13</v>
       </c>
@@ -6820,7 +7899,7 @@
         <v>&lt;0.01</v>
       </c>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>13</v>
       </c>
@@ -6871,7 +7950,7 @@
         <v>&lt;0.0001</v>
       </c>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>13</v>
       </c>
@@ -6922,7 +8001,7 @@
         <v>0.19800000000000001</v>
       </c>
     </row>
-    <row r="142" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>13</v>
       </c>
@@ -6973,7 +8052,7 @@
         <v>&lt;0.001</v>
       </c>
     </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
         <v>13</v>
       </c>
@@ -7024,7 +8103,7 @@
         <v>0.41299999999999998</v>
       </c>
     </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:20" x14ac:dyDescent="0.25">
       <c r="K144" s="60"/>
       <c r="L144" s="60"/>
       <c r="M144" s="60"/>

</xml_diff>